<commit_message>
updates to population list
</commit_message>
<xml_diff>
--- a/Mouse_workbooks/CD_151218_C.xlsx
+++ b/Mouse_workbooks/CD_151218_C.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glickfeld_lab\Documents\docubase\Mouse_workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charlie\Documents\SourceTree_local\docubase\Mouse_workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14895" windowHeight="9315" tabRatio="738"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="14895" windowHeight="9315" tabRatio="738" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="111">
   <si>
     <t>Mouse ID</t>
   </si>
@@ -433,6 +433,18 @@
   </si>
   <si>
     <t>AAV2/1.CAGGS.flex.ChR2.tdtomato. LFP and FV analysis</t>
+  </si>
+  <si>
+    <t>2016_01_11_concat_6and7</t>
+  </si>
+  <si>
+    <t>2016_01_11_concat10and11</t>
+  </si>
+  <si>
+    <t>2016_01_11_concat_18and19</t>
+  </si>
+  <si>
+    <t>2016_01_11_concat_21and22</t>
   </si>
 </sst>
 </file>
@@ -971,7 +983,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1079,6 +1091,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1568,7 +1595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A2" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1650,16 +1677,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:I4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36:I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.75" style="1" customWidth="1"/>
     <col min="3" max="3" width="6.875" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.125" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.125" style="35" customWidth="1"/>
@@ -1671,34 +1698,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="58" t="s">
+      <c r="B1" s="58"/>
+      <c r="C1" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
       <c r="H1" s="25" t="s">
         <v>30</v>
       </c>
       <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="41" t="s">
+      <c r="B2" s="60"/>
+      <c r="C2" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
       <c r="H2" s="26" t="s">
         <v>30</v>
       </c>
@@ -1707,45 +1734,45 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="45">
+      <c r="B3" s="60"/>
+      <c r="C3" s="50">
         <v>34</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="47"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="52"/>
     </row>
     <row r="4" spans="1:9" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="48" t="s">
+      <c r="B4" s="62"/>
+      <c r="C4" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="51"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="56"/>
     </row>
     <row r="5" spans="1:9" ht="26.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="44"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
     </row>
     <row r="6" spans="1:9" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -1766,11 +1793,11 @@
       <c r="F6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="39"/>
-      <c r="I6" s="40"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="45"/>
     </row>
     <row r="7" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -1791,11 +1818,11 @@
       <c r="F7" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="41" t="s">
+      <c r="G7" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="42"/>
-      <c r="I7" s="43"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="48"/>
     </row>
     <row r="8" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -1816,11 +1843,11 @@
       <c r="F8" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="41" t="s">
+      <c r="G8" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="42"/>
-      <c r="I8" s="43"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="48"/>
     </row>
     <row r="9" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -1841,11 +1868,11 @@
       <c r="F9" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="41" t="s">
+      <c r="G9" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="42"/>
-      <c r="I9" s="43"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="48"/>
     </row>
     <row r="10" spans="1:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -1866,11 +1893,11 @@
       <c r="F10" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="41" t="s">
+      <c r="G10" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="42"/>
-      <c r="I10" s="43"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="48"/>
     </row>
     <row r="11" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -1891,11 +1918,11 @@
       <c r="F11" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="41" t="s">
+      <c r="G11" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="H11" s="42"/>
-      <c r="I11" s="43"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="48"/>
     </row>
     <row r="12" spans="1:9" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -1916,11 +1943,11 @@
       <c r="F12" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="41" t="s">
+      <c r="G12" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="42"/>
-      <c r="I12" s="43"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="48"/>
     </row>
     <row r="13" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -1939,11 +1966,11 @@
       <c r="F13" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="41" t="s">
+      <c r="G13" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="42"/>
-      <c r="I13" s="43"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="48"/>
     </row>
     <row r="14" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
@@ -1952,9 +1979,9 @@
       <c r="D14" s="5"/>
       <c r="E14" s="36"/>
       <c r="F14" s="23"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="43"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="48"/>
     </row>
     <row r="15" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -1975,11 +2002,11 @@
       <c r="F15" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="41" t="s">
+      <c r="G15" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="H15" s="42"/>
-      <c r="I15" s="43"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="48"/>
     </row>
     <row r="16" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -2000,11 +2027,11 @@
       <c r="F16" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="41" t="s">
+      <c r="G16" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="H16" s="42"/>
-      <c r="I16" s="43"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="48"/>
     </row>
     <row r="17" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
@@ -2025,11 +2052,11 @@
       <c r="F17" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G17" s="41" t="s">
+      <c r="G17" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="H17" s="42"/>
-      <c r="I17" s="43"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="48"/>
     </row>
     <row r="18" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -2050,11 +2077,11 @@
       <c r="F18" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G18" s="41" t="s">
+      <c r="G18" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="H18" s="42"/>
-      <c r="I18" s="43"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="48"/>
     </row>
     <row r="19" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
@@ -2075,11 +2102,11 @@
       <c r="F19" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="41" t="s">
+      <c r="G19" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="H19" s="42"/>
-      <c r="I19" s="43"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="48"/>
     </row>
     <row r="20" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
@@ -2100,11 +2127,11 @@
       <c r="F20" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="41" t="s">
+      <c r="G20" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="H20" s="42"/>
-      <c r="I20" s="43"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="48"/>
     </row>
     <row r="21" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
@@ -2125,11 +2152,11 @@
       <c r="F21" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G21" s="41" t="s">
+      <c r="G21" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="H21" s="42"/>
-      <c r="I21" s="43"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="48"/>
     </row>
     <row r="22" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
@@ -2150,11 +2177,11 @@
       <c r="F22" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="41" t="s">
+      <c r="G22" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="H22" s="42"/>
-      <c r="I22" s="43"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="48"/>
     </row>
     <row r="23" spans="1:9" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
@@ -2175,11 +2202,11 @@
       <c r="F23" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G23" s="41" t="s">
+      <c r="G23" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="H23" s="42"/>
-      <c r="I23" s="43"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="48"/>
     </row>
     <row r="24" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
@@ -2200,11 +2227,11 @@
       <c r="F24" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G24" s="41" t="s">
+      <c r="G24" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="H24" s="42"/>
-      <c r="I24" s="43"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="48"/>
     </row>
     <row r="25" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
@@ -2225,11 +2252,11 @@
       <c r="F25" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G25" s="41" t="s">
+      <c r="G25" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="H25" s="42"/>
-      <c r="I25" s="43"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="48"/>
     </row>
     <row r="26" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
@@ -2250,58 +2277,68 @@
       <c r="F26" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="41" t="s">
+      <c r="G26" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="H26" s="42"/>
-      <c r="I26" s="43"/>
-    </row>
-    <row r="27" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H26" s="47"/>
+      <c r="I26" s="48"/>
+    </row>
+    <row r="27" spans="1:9" s="41" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>2</v>
       </c>
-      <c r="B27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="C27" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="37">
+      <c r="D27" s="42">
         <v>7</v>
       </c>
-      <c r="E27" s="37">
+      <c r="E27" s="42">
         <v>34</v>
       </c>
-      <c r="F27" s="37" t="s">
+      <c r="F27" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="G27" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="H27" s="42"/>
-      <c r="I27" s="43"/>
-    </row>
-    <row r="28" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="43"/>
-    </row>
-    <row r="29" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G27" s="38"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="40"/>
+    </row>
+    <row r="28" spans="1:9" s="41" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>2</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="42">
+        <v>7</v>
+      </c>
+      <c r="E28" s="42">
+        <v>34</v>
+      </c>
+      <c r="F28" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="38"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="40"/>
+    </row>
+    <row r="29" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>3</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>72</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
         <v>43</v>
       </c>
       <c r="D29" s="37">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E29" s="37">
         <v>34</v>
@@ -2309,43 +2346,29 @@
       <c r="F29" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G29" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="H29" s="42"/>
-      <c r="I29" s="43"/>
-    </row>
-    <row r="30" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>3</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="37">
-        <v>8</v>
-      </c>
-      <c r="E30" s="37">
-        <v>34</v>
-      </c>
-      <c r="F30" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="G30" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="H30" s="42"/>
-      <c r="I30" s="43"/>
-    </row>
-    <row r="31" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G29" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="H29" s="47"/>
+      <c r="I29" s="48"/>
+    </row>
+    <row r="30" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="48"/>
+    </row>
+    <row r="31" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>3</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>43</v>
@@ -2359,18 +2382,18 @@
       <c r="F31" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G31" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="H31" s="42"/>
-      <c r="I31" s="43"/>
-    </row>
-    <row r="32" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G31" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="H31" s="47"/>
+      <c r="I31" s="48"/>
+    </row>
+    <row r="32" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>3</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>43</v>
@@ -2384,18 +2407,18 @@
       <c r="F32" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G32" s="41" t="s">
-        <v>88</v>
-      </c>
-      <c r="H32" s="42"/>
-      <c r="I32" s="43"/>
-    </row>
-    <row r="33" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G32" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="H32" s="47"/>
+      <c r="I32" s="48"/>
+    </row>
+    <row r="33" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>3</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>43</v>
@@ -2409,18 +2432,18 @@
       <c r="F33" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G33" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="H33" s="42"/>
-      <c r="I33" s="43"/>
-    </row>
-    <row r="34" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G33" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="H33" s="47"/>
+      <c r="I33" s="48"/>
+    </row>
+    <row r="34" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>3</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>43</v>
@@ -2434,18 +2457,18 @@
       <c r="F34" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="H34" s="42"/>
-      <c r="I34" s="43"/>
-    </row>
-    <row r="35" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G34" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="H34" s="47"/>
+      <c r="I34" s="48"/>
+    </row>
+    <row r="35" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>3</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>43</v>
@@ -2459,18 +2482,18 @@
       <c r="F35" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G35" s="41" t="s">
-        <v>95</v>
-      </c>
-      <c r="H35" s="42"/>
-      <c r="I35" s="43"/>
-    </row>
-    <row r="36" spans="1:9" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G35" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="H35" s="47"/>
+      <c r="I35" s="48"/>
+    </row>
+    <row r="36" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>3</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>43</v>
@@ -2484,18 +2507,18 @@
       <c r="F36" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G36" s="41" t="s">
-        <v>96</v>
-      </c>
-      <c r="H36" s="42"/>
-      <c r="I36" s="43"/>
-    </row>
-    <row r="37" spans="1:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G36" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="H36" s="47"/>
+      <c r="I36" s="48"/>
+    </row>
+    <row r="37" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>3</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>43</v>
@@ -2509,18 +2532,18 @@
       <c r="F37" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G37" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="H37" s="42"/>
-      <c r="I37" s="43"/>
-    </row>
-    <row r="38" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G37" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="H37" s="47"/>
+      <c r="I37" s="48"/>
+    </row>
+    <row r="38" spans="1:9" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>3</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>43</v>
@@ -2534,17 +2557,19 @@
       <c r="F38" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G38" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="H38" s="42"/>
-      <c r="I38" s="43"/>
-    </row>
-    <row r="39" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G38" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="H38" s="47"/>
+      <c r="I38" s="48"/>
+    </row>
+    <row r="39" spans="1:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>3</v>
       </c>
-      <c r="B39" s="4"/>
+      <c r="B39" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="C39" s="4" t="s">
         <v>43</v>
       </c>
@@ -2557,66 +2582,116 @@
       <c r="F39" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G39" s="41" t="s">
+      <c r="G39" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="H39" s="47"/>
+      <c r="I39" s="48"/>
+    </row>
+    <row r="40" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>3</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" s="37">
+        <v>8</v>
+      </c>
+      <c r="E40" s="37">
+        <v>34</v>
+      </c>
+      <c r="F40" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="G40" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="H40" s="47"/>
+      <c r="I40" s="48"/>
+    </row>
+    <row r="41" spans="1:9" s="41" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>3</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" s="42">
+        <v>8</v>
+      </c>
+      <c r="E41" s="42">
+        <v>34</v>
+      </c>
+      <c r="F41" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="G41" s="38"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="40"/>
+    </row>
+    <row r="42" spans="1:9" s="41" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>3</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" s="42">
+        <v>8</v>
+      </c>
+      <c r="E42" s="42">
+        <v>34</v>
+      </c>
+      <c r="F42" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="G42" s="38"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="40"/>
+    </row>
+    <row r="43" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>3</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" s="37">
+        <v>8</v>
+      </c>
+      <c r="E43" s="37">
+        <v>34</v>
+      </c>
+      <c r="F43" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="G43" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="H39" s="42"/>
-      <c r="I39" s="43"/>
-    </row>
-    <row r="40" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="41"/>
-      <c r="H40" s="42"/>
-      <c r="I40" s="43"/>
-    </row>
-    <row r="41" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="43"/>
-    </row>
-    <row r="42" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="41"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="43"/>
-    </row>
-    <row r="43" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="41"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="43"/>
+      <c r="H43" s="47"/>
+      <c r="I43" s="48"/>
     </row>
     <row r="44" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="41"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="43"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="46"/>
+      <c r="H44" s="47"/>
+      <c r="I44" s="48"/>
     </row>
     <row r="45" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
@@ -2625,9 +2700,9 @@
       <c r="D45" s="5"/>
       <c r="E45" s="36"/>
       <c r="F45" s="23"/>
-      <c r="G45" s="41"/>
-      <c r="H45" s="42"/>
-      <c r="I45" s="43"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="47"/>
+      <c r="I45" s="48"/>
     </row>
     <row r="46" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
@@ -2636,9 +2711,9 @@
       <c r="D46" s="5"/>
       <c r="E46" s="36"/>
       <c r="F46" s="23"/>
-      <c r="G46" s="41"/>
-      <c r="H46" s="42"/>
-      <c r="I46" s="43"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="47"/>
+      <c r="I46" s="48"/>
     </row>
     <row r="47" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
@@ -2647,9 +2722,9 @@
       <c r="D47" s="5"/>
       <c r="E47" s="36"/>
       <c r="F47" s="23"/>
-      <c r="G47" s="41"/>
-      <c r="H47" s="42"/>
-      <c r="I47" s="43"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="47"/>
+      <c r="I47" s="48"/>
     </row>
     <row r="48" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
@@ -2658,9 +2733,9 @@
       <c r="D48" s="5"/>
       <c r="E48" s="36"/>
       <c r="F48" s="23"/>
-      <c r="G48" s="41"/>
-      <c r="H48" s="42"/>
-      <c r="I48" s="43"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="47"/>
+      <c r="I48" s="48"/>
     </row>
     <row r="49" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
@@ -2669,9 +2744,9 @@
       <c r="D49" s="5"/>
       <c r="E49" s="36"/>
       <c r="F49" s="23"/>
-      <c r="G49" s="41"/>
-      <c r="H49" s="42"/>
-      <c r="I49" s="43"/>
+      <c r="G49" s="46"/>
+      <c r="H49" s="47"/>
+      <c r="I49" s="48"/>
     </row>
     <row r="50" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
@@ -2680,9 +2755,9 @@
       <c r="D50" s="5"/>
       <c r="E50" s="36"/>
       <c r="F50" s="23"/>
-      <c r="G50" s="41"/>
-      <c r="H50" s="42"/>
-      <c r="I50" s="43"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="47"/>
+      <c r="I50" s="48"/>
     </row>
     <row r="51" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
@@ -2691,9 +2766,9 @@
       <c r="D51" s="5"/>
       <c r="E51" s="36"/>
       <c r="F51" s="23"/>
-      <c r="G51" s="41"/>
-      <c r="H51" s="42"/>
-      <c r="I51" s="43"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="47"/>
+      <c r="I51" s="48"/>
     </row>
     <row r="52" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
@@ -2702,9 +2777,9 @@
       <c r="D52" s="5"/>
       <c r="E52" s="36"/>
       <c r="F52" s="23"/>
-      <c r="G52" s="41"/>
-      <c r="H52" s="42"/>
-      <c r="I52" s="43"/>
+      <c r="G52" s="46"/>
+      <c r="H52" s="47"/>
+      <c r="I52" s="48"/>
     </row>
     <row r="53" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
@@ -2713,9 +2788,9 @@
       <c r="D53" s="5"/>
       <c r="E53" s="36"/>
       <c r="F53" s="23"/>
-      <c r="G53" s="41"/>
-      <c r="H53" s="42"/>
-      <c r="I53" s="43"/>
+      <c r="G53" s="46"/>
+      <c r="H53" s="47"/>
+      <c r="I53" s="48"/>
     </row>
     <row r="54" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
@@ -2724,9 +2799,9 @@
       <c r="D54" s="5"/>
       <c r="E54" s="36"/>
       <c r="F54" s="23"/>
-      <c r="G54" s="41"/>
-      <c r="H54" s="42"/>
-      <c r="I54" s="43"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="47"/>
+      <c r="I54" s="48"/>
     </row>
     <row r="55" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
@@ -2735,9 +2810,9 @@
       <c r="D55" s="5"/>
       <c r="E55" s="36"/>
       <c r="F55" s="23"/>
-      <c r="G55" s="41"/>
-      <c r="H55" s="42"/>
-      <c r="I55" s="43"/>
+      <c r="G55" s="46"/>
+      <c r="H55" s="47"/>
+      <c r="I55" s="48"/>
     </row>
     <row r="56" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
@@ -2746,9 +2821,9 @@
       <c r="D56" s="5"/>
       <c r="E56" s="36"/>
       <c r="F56" s="23"/>
-      <c r="G56" s="41"/>
-      <c r="H56" s="42"/>
-      <c r="I56" s="43"/>
+      <c r="G56" s="46"/>
+      <c r="H56" s="47"/>
+      <c r="I56" s="48"/>
     </row>
     <row r="57" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
@@ -2757,9 +2832,9 @@
       <c r="D57" s="5"/>
       <c r="E57" s="36"/>
       <c r="F57" s="23"/>
-      <c r="G57" s="41"/>
-      <c r="H57" s="42"/>
-      <c r="I57" s="43"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="47"/>
+      <c r="I57" s="48"/>
     </row>
     <row r="58" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
@@ -2768,9 +2843,9 @@
       <c r="D58" s="5"/>
       <c r="E58" s="36"/>
       <c r="F58" s="23"/>
-      <c r="G58" s="41"/>
-      <c r="H58" s="42"/>
-      <c r="I58" s="43"/>
+      <c r="G58" s="46"/>
+      <c r="H58" s="47"/>
+      <c r="I58" s="48"/>
     </row>
     <row r="59" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
@@ -2779,9 +2854,9 @@
       <c r="D59" s="5"/>
       <c r="E59" s="36"/>
       <c r="F59" s="23"/>
-      <c r="G59" s="41"/>
-      <c r="H59" s="42"/>
-      <c r="I59" s="43"/>
+      <c r="G59" s="46"/>
+      <c r="H59" s="47"/>
+      <c r="I59" s="48"/>
     </row>
     <row r="60" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
@@ -2790,9 +2865,9 @@
       <c r="D60" s="5"/>
       <c r="E60" s="36"/>
       <c r="F60" s="23"/>
-      <c r="G60" s="41"/>
-      <c r="H60" s="42"/>
-      <c r="I60" s="43"/>
+      <c r="G60" s="46"/>
+      <c r="H60" s="47"/>
+      <c r="I60" s="48"/>
     </row>
     <row r="61" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
@@ -2801,9 +2876,9 @@
       <c r="D61" s="5"/>
       <c r="E61" s="36"/>
       <c r="F61" s="23"/>
-      <c r="G61" s="41"/>
-      <c r="H61" s="42"/>
-      <c r="I61" s="43"/>
+      <c r="G61" s="46"/>
+      <c r="H61" s="47"/>
+      <c r="I61" s="48"/>
     </row>
     <row r="62" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
@@ -2812,9 +2887,9 @@
       <c r="D62" s="5"/>
       <c r="E62" s="36"/>
       <c r="F62" s="23"/>
-      <c r="G62" s="41"/>
-      <c r="H62" s="42"/>
-      <c r="I62" s="43"/>
+      <c r="G62" s="46"/>
+      <c r="H62" s="47"/>
+      <c r="I62" s="48"/>
     </row>
     <row r="63" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
@@ -2823,9 +2898,9 @@
       <c r="D63" s="5"/>
       <c r="E63" s="36"/>
       <c r="F63" s="23"/>
-      <c r="G63" s="41"/>
-      <c r="H63" s="42"/>
-      <c r="I63" s="43"/>
+      <c r="G63" s="46"/>
+      <c r="H63" s="47"/>
+      <c r="I63" s="48"/>
     </row>
     <row r="64" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
@@ -2834,9 +2909,9 @@
       <c r="D64" s="5"/>
       <c r="E64" s="36"/>
       <c r="F64" s="23"/>
-      <c r="G64" s="41"/>
-      <c r="H64" s="42"/>
-      <c r="I64" s="43"/>
+      <c r="G64" s="46"/>
+      <c r="H64" s="47"/>
+      <c r="I64" s="48"/>
     </row>
     <row r="65" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
@@ -2845,9 +2920,9 @@
       <c r="D65" s="5"/>
       <c r="E65" s="36"/>
       <c r="F65" s="23"/>
-      <c r="G65" s="41"/>
-      <c r="H65" s="42"/>
-      <c r="I65" s="43"/>
+      <c r="G65" s="46"/>
+      <c r="H65" s="47"/>
+      <c r="I65" s="48"/>
     </row>
     <row r="66" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
@@ -2856,9 +2931,9 @@
       <c r="D66" s="5"/>
       <c r="E66" s="36"/>
       <c r="F66" s="23"/>
-      <c r="G66" s="41"/>
-      <c r="H66" s="42"/>
-      <c r="I66" s="43"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="47"/>
+      <c r="I66" s="48"/>
     </row>
     <row r="67" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
@@ -2867,9 +2942,9 @@
       <c r="D67" s="5"/>
       <c r="E67" s="36"/>
       <c r="F67" s="23"/>
-      <c r="G67" s="41"/>
-      <c r="H67" s="42"/>
-      <c r="I67" s="43"/>
+      <c r="G67" s="46"/>
+      <c r="H67" s="47"/>
+      <c r="I67" s="48"/>
     </row>
     <row r="68" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
@@ -2878,9 +2953,9 @@
       <c r="D68" s="5"/>
       <c r="E68" s="36"/>
       <c r="F68" s="23"/>
-      <c r="G68" s="41"/>
-      <c r="H68" s="42"/>
-      <c r="I68" s="43"/>
+      <c r="G68" s="46"/>
+      <c r="H68" s="47"/>
+      <c r="I68" s="48"/>
     </row>
     <row r="69" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
@@ -2889,9 +2964,9 @@
       <c r="D69" s="5"/>
       <c r="E69" s="36"/>
       <c r="F69" s="23"/>
-      <c r="G69" s="41"/>
-      <c r="H69" s="42"/>
-      <c r="I69" s="43"/>
+      <c r="G69" s="46"/>
+      <c r="H69" s="47"/>
+      <c r="I69" s="48"/>
     </row>
     <row r="70" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
@@ -2900,9 +2975,9 @@
       <c r="D70" s="5"/>
       <c r="E70" s="36"/>
       <c r="F70" s="23"/>
-      <c r="G70" s="41"/>
-      <c r="H70" s="42"/>
-      <c r="I70" s="43"/>
+      <c r="G70" s="46"/>
+      <c r="H70" s="47"/>
+      <c r="I70" s="48"/>
     </row>
     <row r="71" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
@@ -2911,9 +2986,9 @@
       <c r="D71" s="5"/>
       <c r="E71" s="36"/>
       <c r="F71" s="23"/>
-      <c r="G71" s="41"/>
-      <c r="H71" s="42"/>
-      <c r="I71" s="43"/>
+      <c r="G71" s="46"/>
+      <c r="H71" s="47"/>
+      <c r="I71" s="48"/>
     </row>
     <row r="72" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
@@ -2922,9 +2997,9 @@
       <c r="D72" s="5"/>
       <c r="E72" s="36"/>
       <c r="F72" s="23"/>
-      <c r="G72" s="41"/>
-      <c r="H72" s="42"/>
-      <c r="I72" s="43"/>
+      <c r="G72" s="46"/>
+      <c r="H72" s="47"/>
+      <c r="I72" s="48"/>
     </row>
     <row r="73" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
@@ -2933,9 +3008,9 @@
       <c r="D73" s="5"/>
       <c r="E73" s="36"/>
       <c r="F73" s="23"/>
-      <c r="G73" s="41"/>
-      <c r="H73" s="42"/>
-      <c r="I73" s="43"/>
+      <c r="G73" s="46"/>
+      <c r="H73" s="47"/>
+      <c r="I73" s="48"/>
     </row>
     <row r="74" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
@@ -2944,9 +3019,9 @@
       <c r="D74" s="5"/>
       <c r="E74" s="36"/>
       <c r="F74" s="23"/>
-      <c r="G74" s="41"/>
-      <c r="H74" s="42"/>
-      <c r="I74" s="43"/>
+      <c r="G74" s="46"/>
+      <c r="H74" s="47"/>
+      <c r="I74" s="48"/>
     </row>
     <row r="75" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
@@ -2955,9 +3030,9 @@
       <c r="D75" s="5"/>
       <c r="E75" s="36"/>
       <c r="F75" s="23"/>
-      <c r="G75" s="41"/>
-      <c r="H75" s="42"/>
-      <c r="I75" s="43"/>
+      <c r="G75" s="46"/>
+      <c r="H75" s="47"/>
+      <c r="I75" s="48"/>
     </row>
     <row r="76" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
@@ -2966,9 +3041,9 @@
       <c r="D76" s="5"/>
       <c r="E76" s="36"/>
       <c r="F76" s="23"/>
-      <c r="G76" s="41"/>
-      <c r="H76" s="42"/>
-      <c r="I76" s="43"/>
+      <c r="G76" s="46"/>
+      <c r="H76" s="47"/>
+      <c r="I76" s="48"/>
     </row>
     <row r="77" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
@@ -2977,9 +3052,9 @@
       <c r="D77" s="5"/>
       <c r="E77" s="36"/>
       <c r="F77" s="23"/>
-      <c r="G77" s="41"/>
-      <c r="H77" s="42"/>
-      <c r="I77" s="43"/>
+      <c r="G77" s="46"/>
+      <c r="H77" s="47"/>
+      <c r="I77" s="48"/>
     </row>
     <row r="78" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
@@ -2988,9 +3063,9 @@
       <c r="D78" s="5"/>
       <c r="E78" s="36"/>
       <c r="F78" s="23"/>
-      <c r="G78" s="41"/>
-      <c r="H78" s="42"/>
-      <c r="I78" s="43"/>
+      <c r="G78" s="46"/>
+      <c r="H78" s="47"/>
+      <c r="I78" s="48"/>
     </row>
     <row r="79" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
@@ -2999,9 +3074,9 @@
       <c r="D79" s="5"/>
       <c r="E79" s="36"/>
       <c r="F79" s="23"/>
-      <c r="G79" s="41"/>
-      <c r="H79" s="42"/>
-      <c r="I79" s="43"/>
+      <c r="G79" s="46"/>
+      <c r="H79" s="47"/>
+      <c r="I79" s="48"/>
     </row>
     <row r="80" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
@@ -3010,9 +3085,9 @@
       <c r="D80" s="5"/>
       <c r="E80" s="36"/>
       <c r="F80" s="23"/>
-      <c r="G80" s="41"/>
-      <c r="H80" s="42"/>
-      <c r="I80" s="43"/>
+      <c r="G80" s="46"/>
+      <c r="H80" s="47"/>
+      <c r="I80" s="48"/>
     </row>
     <row r="81" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
@@ -3021,9 +3096,9 @@
       <c r="D81" s="5"/>
       <c r="E81" s="36"/>
       <c r="F81" s="23"/>
-      <c r="G81" s="41"/>
-      <c r="H81" s="42"/>
-      <c r="I81" s="43"/>
+      <c r="G81" s="46"/>
+      <c r="H81" s="47"/>
+      <c r="I81" s="48"/>
     </row>
     <row r="82" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
@@ -3032,9 +3107,9 @@
       <c r="D82" s="5"/>
       <c r="E82" s="36"/>
       <c r="F82" s="23"/>
-      <c r="G82" s="41"/>
-      <c r="H82" s="42"/>
-      <c r="I82" s="43"/>
+      <c r="G82" s="46"/>
+      <c r="H82" s="47"/>
+      <c r="I82" s="48"/>
     </row>
     <row r="83" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
@@ -3043,9 +3118,9 @@
       <c r="D83" s="5"/>
       <c r="E83" s="36"/>
       <c r="F83" s="23"/>
-      <c r="G83" s="41"/>
-      <c r="H83" s="42"/>
-      <c r="I83" s="43"/>
+      <c r="G83" s="46"/>
+      <c r="H83" s="47"/>
+      <c r="I83" s="48"/>
     </row>
     <row r="84" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
@@ -3054,9 +3129,9 @@
       <c r="D84" s="5"/>
       <c r="E84" s="36"/>
       <c r="F84" s="23"/>
-      <c r="G84" s="41"/>
-      <c r="H84" s="42"/>
-      <c r="I84" s="43"/>
+      <c r="G84" s="46"/>
+      <c r="H84" s="47"/>
+      <c r="I84" s="48"/>
     </row>
     <row r="85" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
@@ -3065,9 +3140,9 @@
       <c r="D85" s="5"/>
       <c r="E85" s="36"/>
       <c r="F85" s="23"/>
-      <c r="G85" s="41"/>
-      <c r="H85" s="42"/>
-      <c r="I85" s="43"/>
+      <c r="G85" s="46"/>
+      <c r="H85" s="47"/>
+      <c r="I85" s="48"/>
     </row>
     <row r="86" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
@@ -3076,9 +3151,9 @@
       <c r="D86" s="5"/>
       <c r="E86" s="36"/>
       <c r="F86" s="23"/>
-      <c r="G86" s="41"/>
-      <c r="H86" s="42"/>
-      <c r="I86" s="43"/>
+      <c r="G86" s="46"/>
+      <c r="H86" s="47"/>
+      <c r="I86" s="48"/>
     </row>
     <row r="87" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
@@ -3087,9 +3162,9 @@
       <c r="D87" s="5"/>
       <c r="E87" s="36"/>
       <c r="F87" s="23"/>
-      <c r="G87" s="41"/>
-      <c r="H87" s="42"/>
-      <c r="I87" s="43"/>
+      <c r="G87" s="46"/>
+      <c r="H87" s="47"/>
+      <c r="I87" s="48"/>
     </row>
     <row r="88" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
@@ -3098,9 +3173,9 @@
       <c r="D88" s="5"/>
       <c r="E88" s="36"/>
       <c r="F88" s="23"/>
-      <c r="G88" s="41"/>
-      <c r="H88" s="42"/>
-      <c r="I88" s="43"/>
+      <c r="G88" s="46"/>
+      <c r="H88" s="47"/>
+      <c r="I88" s="48"/>
     </row>
     <row r="89" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
@@ -3109,9 +3184,9 @@
       <c r="D89" s="5"/>
       <c r="E89" s="36"/>
       <c r="F89" s="23"/>
-      <c r="G89" s="41"/>
-      <c r="H89" s="42"/>
-      <c r="I89" s="43"/>
+      <c r="G89" s="46"/>
+      <c r="H89" s="47"/>
+      <c r="I89" s="48"/>
     </row>
     <row r="90" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
@@ -3120,9 +3195,9 @@
       <c r="D90" s="5"/>
       <c r="E90" s="36"/>
       <c r="F90" s="23"/>
-      <c r="G90" s="41"/>
-      <c r="H90" s="42"/>
-      <c r="I90" s="43"/>
+      <c r="G90" s="46"/>
+      <c r="H90" s="47"/>
+      <c r="I90" s="48"/>
     </row>
     <row r="91" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
@@ -3131,9 +3206,9 @@
       <c r="D91" s="5"/>
       <c r="E91" s="36"/>
       <c r="F91" s="23"/>
-      <c r="G91" s="41"/>
-      <c r="H91" s="42"/>
-      <c r="I91" s="43"/>
+      <c r="G91" s="46"/>
+      <c r="H91" s="47"/>
+      <c r="I91" s="48"/>
     </row>
     <row r="92" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
@@ -3142,9 +3217,9 @@
       <c r="D92" s="5"/>
       <c r="E92" s="36"/>
       <c r="F92" s="23"/>
-      <c r="G92" s="41"/>
-      <c r="H92" s="42"/>
-      <c r="I92" s="43"/>
+      <c r="G92" s="46"/>
+      <c r="H92" s="47"/>
+      <c r="I92" s="48"/>
     </row>
     <row r="93" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
@@ -3153,9 +3228,9 @@
       <c r="D93" s="5"/>
       <c r="E93" s="36"/>
       <c r="F93" s="23"/>
-      <c r="G93" s="41"/>
-      <c r="H93" s="42"/>
-      <c r="I93" s="43"/>
+      <c r="G93" s="46"/>
+      <c r="H93" s="47"/>
+      <c r="I93" s="48"/>
     </row>
     <row r="94" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
@@ -3164,9 +3239,9 @@
       <c r="D94" s="5"/>
       <c r="E94" s="36"/>
       <c r="F94" s="23"/>
-      <c r="G94" s="41"/>
-      <c r="H94" s="42"/>
-      <c r="I94" s="43"/>
+      <c r="G94" s="46"/>
+      <c r="H94" s="47"/>
+      <c r="I94" s="48"/>
     </row>
     <row r="95" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
@@ -3175,9 +3250,9 @@
       <c r="D95" s="5"/>
       <c r="E95" s="36"/>
       <c r="F95" s="23"/>
-      <c r="G95" s="41"/>
-      <c r="H95" s="42"/>
-      <c r="I95" s="43"/>
+      <c r="G95" s="46"/>
+      <c r="H95" s="47"/>
+      <c r="I95" s="48"/>
     </row>
     <row r="96" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
@@ -3186,9 +3261,9 @@
       <c r="D96" s="5"/>
       <c r="E96" s="36"/>
       <c r="F96" s="23"/>
-      <c r="G96" s="41"/>
-      <c r="H96" s="42"/>
-      <c r="I96" s="43"/>
+      <c r="G96" s="46"/>
+      <c r="H96" s="47"/>
+      <c r="I96" s="48"/>
     </row>
     <row r="97" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
@@ -3197,9 +3272,9 @@
       <c r="D97" s="5"/>
       <c r="E97" s="36"/>
       <c r="F97" s="23"/>
-      <c r="G97" s="41"/>
-      <c r="H97" s="42"/>
-      <c r="I97" s="43"/>
+      <c r="G97" s="46"/>
+      <c r="H97" s="47"/>
+      <c r="I97" s="48"/>
     </row>
     <row r="98" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
@@ -3208,9 +3283,9 @@
       <c r="D98" s="5"/>
       <c r="E98" s="36"/>
       <c r="F98" s="23"/>
-      <c r="G98" s="41"/>
-      <c r="H98" s="42"/>
-      <c r="I98" s="43"/>
+      <c r="G98" s="46"/>
+      <c r="H98" s="47"/>
+      <c r="I98" s="48"/>
     </row>
     <row r="99" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
@@ -3219,9 +3294,9 @@
       <c r="D99" s="5"/>
       <c r="E99" s="36"/>
       <c r="F99" s="23"/>
-      <c r="G99" s="41"/>
-      <c r="H99" s="42"/>
-      <c r="I99" s="43"/>
+      <c r="G99" s="46"/>
+      <c r="H99" s="47"/>
+      <c r="I99" s="48"/>
     </row>
     <row r="100" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
@@ -3230,88 +3305,132 @@
       <c r="D100" s="5"/>
       <c r="E100" s="36"/>
       <c r="F100" s="23"/>
-      <c r="G100" s="41"/>
-      <c r="H100" s="42"/>
-      <c r="I100" s="43"/>
-    </row>
-    <row r="101" spans="1:9" ht="39" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="G100" s="46"/>
+      <c r="H100" s="47"/>
+      <c r="I100" s="48"/>
+    </row>
+    <row r="101" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="3"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="36"/>
+      <c r="F101" s="23"/>
+      <c r="G101" s="46"/>
+      <c r="H101" s="47"/>
+      <c r="I101" s="48"/>
+    </row>
+    <row r="102" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="36"/>
+      <c r="F102" s="23"/>
+      <c r="G102" s="46"/>
+      <c r="H102" s="47"/>
+      <c r="I102" s="48"/>
+    </row>
+    <row r="103" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="3"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="36"/>
+      <c r="F103" s="23"/>
+      <c r="G103" s="46"/>
+      <c r="H103" s="47"/>
+      <c r="I103" s="48"/>
+    </row>
+    <row r="104" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="36"/>
+      <c r="F104" s="23"/>
+      <c r="G104" s="46"/>
+      <c r="H104" s="47"/>
+      <c r="I104" s="48"/>
+    </row>
+    <row r="105" spans="1:9" ht="39" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="104">
+    <mergeCell ref="G100:I100"/>
+    <mergeCell ref="G101:I101"/>
+    <mergeCell ref="G102:I102"/>
+    <mergeCell ref="G103:I103"/>
+    <mergeCell ref="G104:I104"/>
+    <mergeCell ref="G95:I95"/>
     <mergeCell ref="G96:I96"/>
     <mergeCell ref="G97:I97"/>
     <mergeCell ref="G98:I98"/>
     <mergeCell ref="G99:I99"/>
-    <mergeCell ref="G100:I100"/>
+    <mergeCell ref="G90:I90"/>
     <mergeCell ref="G91:I91"/>
     <mergeCell ref="G92:I92"/>
     <mergeCell ref="G93:I93"/>
     <mergeCell ref="G94:I94"/>
-    <mergeCell ref="G95:I95"/>
+    <mergeCell ref="G85:I85"/>
     <mergeCell ref="G86:I86"/>
     <mergeCell ref="G87:I87"/>
     <mergeCell ref="G88:I88"/>
     <mergeCell ref="G89:I89"/>
-    <mergeCell ref="G90:I90"/>
+    <mergeCell ref="G80:I80"/>
     <mergeCell ref="G81:I81"/>
     <mergeCell ref="G82:I82"/>
     <mergeCell ref="G83:I83"/>
     <mergeCell ref="G84:I84"/>
-    <mergeCell ref="G85:I85"/>
+    <mergeCell ref="G75:I75"/>
     <mergeCell ref="G76:I76"/>
     <mergeCell ref="G77:I77"/>
     <mergeCell ref="G78:I78"/>
     <mergeCell ref="G79:I79"/>
-    <mergeCell ref="G80:I80"/>
+    <mergeCell ref="G70:I70"/>
     <mergeCell ref="G71:I71"/>
     <mergeCell ref="G72:I72"/>
     <mergeCell ref="G73:I73"/>
     <mergeCell ref="G74:I74"/>
-    <mergeCell ref="G75:I75"/>
+    <mergeCell ref="G65:I65"/>
     <mergeCell ref="G66:I66"/>
     <mergeCell ref="G67:I67"/>
     <mergeCell ref="G68:I68"/>
     <mergeCell ref="G69:I69"/>
-    <mergeCell ref="G70:I70"/>
+    <mergeCell ref="G60:I60"/>
     <mergeCell ref="G61:I61"/>
     <mergeCell ref="G62:I62"/>
     <mergeCell ref="G63:I63"/>
     <mergeCell ref="G64:I64"/>
-    <mergeCell ref="G65:I65"/>
+    <mergeCell ref="G55:I55"/>
     <mergeCell ref="G56:I56"/>
     <mergeCell ref="G57:I57"/>
     <mergeCell ref="G58:I58"/>
     <mergeCell ref="G59:I59"/>
-    <mergeCell ref="G60:I60"/>
+    <mergeCell ref="G50:I50"/>
     <mergeCell ref="G51:I51"/>
     <mergeCell ref="G52:I52"/>
     <mergeCell ref="G53:I53"/>
     <mergeCell ref="G54:I54"/>
-    <mergeCell ref="G55:I55"/>
+    <mergeCell ref="G45:I45"/>
     <mergeCell ref="G46:I46"/>
     <mergeCell ref="G47:I47"/>
     <mergeCell ref="G48:I48"/>
     <mergeCell ref="G49:I49"/>
-    <mergeCell ref="G50:I50"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="G37:I37"/>
     <mergeCell ref="G38:I38"/>
     <mergeCell ref="G39:I39"/>
     <mergeCell ref="G40:I40"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="G43:I43"/>
+    <mergeCell ref="G44:I44"/>
     <mergeCell ref="G33:I33"/>
     <mergeCell ref="G34:I34"/>
     <mergeCell ref="G35:I35"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="G37:I37"/>
     <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
     <mergeCell ref="G29:I29"/>
     <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="G32:I32"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
     <mergeCell ref="G23:I23"/>
@@ -3373,79 +3492,79 @@
       <c r="A1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="61"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="66"/>
     </row>
     <row r="2" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="63"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="68"/>
     </row>
     <row r="3" spans="1:5" ht="135.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="65"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="70"/>
     </row>
     <row r="4" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="68"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="70"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="75"/>
     </row>
     <row r="5" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="65"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="70"/>
     </row>
     <row r="6" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="65"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="70"/>
     </row>
     <row r="7" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="70"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="75"/>
     </row>
     <row r="8" spans="1:5" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="67"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3486,178 +3605,178 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="73"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="78"/>
     </row>
     <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="74">
+      <c r="B2" s="79">
         <v>42356</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="65"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="70"/>
     </row>
     <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="65"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="70"/>
     </row>
     <row r="4" spans="1:7" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="65"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="70"/>
     </row>
     <row r="5" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="67"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="72"/>
     </row>
     <row r="6" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="73"/>
+      <c r="B7" s="77"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="78"/>
     </row>
     <row r="8" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="76"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="81"/>
     </row>
     <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="64"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="65"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="70"/>
     </row>
     <row r="10" spans="1:7" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="65"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="70"/>
     </row>
     <row r="11" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="77"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="78"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="83"/>
     </row>
     <row r="12" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="71" t="s">
+      <c r="A14" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="73"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="78"/>
     </row>
     <row r="15" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="79"/>
-      <c r="C15" s="79"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="79"/>
-      <c r="G15" s="80"/>
+      <c r="B15" s="84"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="84"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="85"/>
     </row>
     <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="65"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="70"/>
     </row>
     <row r="17" spans="1:7" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="64"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="65"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="70"/>
     </row>
     <row r="18" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="81"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="81"/>
-      <c r="E18" s="81"/>
-      <c r="F18" s="81"/>
-      <c r="G18" s="82"/>
+      <c r="B18" s="86"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="87"/>
     </row>
     <row r="19" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>